<commit_message>
Evo uneseni rezultati za različite značajke.
</commit_message>
<xml_diff>
--- a/dokumentacija/rezultati.xlsx
+++ b/dokumentacija/rezultati.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
-  <si>
-    <t>Baza</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>ismir</t>
   </si>
@@ -61,6 +58,45 @@
   </si>
   <si>
     <t>C=5, linear</t>
+  </si>
+  <si>
+    <t>razl. Baze</t>
+  </si>
+  <si>
+    <t>razl. Značajke</t>
+  </si>
+  <si>
+    <t>značajke</t>
+  </si>
+  <si>
+    <t>broj vrijednosti</t>
+  </si>
+  <si>
+    <t>baza</t>
+  </si>
+  <si>
+    <t>loudness</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>točnost</t>
+  </si>
+  <si>
+    <t>mean, nonzero count</t>
+  </si>
+  <si>
+    <t>mean, nonzero count, loudness</t>
+  </si>
+  <si>
+    <t>mean, nonzero count, loudness, mfcc, spectral_centroid</t>
+  </si>
+  <si>
+    <t>spectral centroid</t>
+  </si>
+  <si>
+    <t>nonzero count</t>
   </si>
 </sst>
 </file>
@@ -97,9 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Obično" xfId="0" builtinId="0"/>
@@ -394,15 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="A1:G4"/>
+      <selection activeCell="C19" sqref="A11:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" customWidth="1"/>
     <col min="5" max="5" width="35.140625" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
@@ -411,85 +449,44 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="G2">
-        <v>39.72</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="G3">
-        <v>36.5</v>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -498,7 +495,157 @@
         <v>0.8</v>
       </c>
       <c r="G4">
+        <v>39.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G5">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G6">
         <v>83.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>63</v>
+      </c>
+      <c r="C12">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>78</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.41499999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodani rezultati u excelu
</commit_message>
<xml_diff>
--- a/dokumentacija/rezultati.xlsx
+++ b/dokumentacija/rezultati.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="28755" windowHeight="12810"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19320" windowHeight="12810"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>ismir</t>
   </si>
@@ -97,6 +97,27 @@
   </si>
   <si>
     <t>nonzero count</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>baza gtzan, broj žanrova 10 (svi), značajka mfcc, klasifikator kresvm(novi), treniranje 80%</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>gama/poli</t>
+  </si>
+  <si>
+    <t>rezultat</t>
+  </si>
+  <si>
+    <t>vrsta kernela</t>
+  </si>
+  <si>
+    <t>linearni (1)</t>
   </si>
 </sst>
 </file>
@@ -139,7 +160,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Obično" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -147,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -431,17 +452,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="A11:C19"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="56.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="35.140625" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="36.85546875" customWidth="1"/>
@@ -615,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -626,7 +648,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -637,7 +659,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -646,6 +668,195 @@
       </c>
       <c r="C19" s="2">
         <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>0.6</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>0.7</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>0.8</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>0.9</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.435</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>1.2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>1.3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38">
+        <v>1.5</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.40500000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.39500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>